<commit_message>
update nova autumn nomination
</commit_message>
<xml_diff>
--- a/data/characters/base/characters-data.xlsx
+++ b/data/characters/base/characters-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ISML\ISML2024-github\data\characters\base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB7F68B-EE83-4771-8BB0-D90795110718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14CC1FC-2799-4054-B198-93E793A7EAF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3191" uniqueCount="2480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3315" uniqueCount="2563">
   <si>
     <t>角色</t>
   </si>
@@ -8398,6 +8398,338 @@
   </si>
   <si>
     <t>Payton尚未</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>猪股大喜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Inomata Taiki</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高仓健</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Takakura Ken</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>田沼要</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tanuma Kaname</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>鸭乃桥论</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>鸭乃桥论的禁忌推理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kamonohashi Ron</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>藤丸立香</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fate系列</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fujimaru Ritsuka</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>早乙女乱马</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Saotome Ranma</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中野丸尾</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>五等分的新娘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nakano Maruo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>多兰</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>再见龙生，你好人生</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dolan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>佐佐木常宏</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sasaki Tsunehiro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>拉法尔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rafal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>圆城寺仁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enjōji Jin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大原拓也</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ōhara Takuya</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>贝尔多尔·贝尔别特·贝尔休伯特</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Veltol Velvet Velsvalt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上终瓜生</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kamihate Uryū</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>踯躅森贵明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tsutsujimori Takaaki</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>花散仁央</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>青之壬生浪</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chirinu Nio</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>哈迪斯·迪奥斯·拉维</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hadis Teos Rave</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>河合井小太郎</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kawaii Kotarō</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>克莱·安东黎希</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>叹气的亡灵想隐退</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Krai Andrey</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新岛圭介</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Niijima Keisuke</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>南云始</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nagumo Hajime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>天束光</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>机械手臂</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Amatsuga Hikaru</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>库洛马</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chrome</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>遥</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>孤单一人的异世界攻略</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Haruka</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>阳务乐郎</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>香格里拉边境～粪作猎人向神作游戏发起挑战～</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hizutome Rakurō</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>五十岚一贺</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>喂！蜻蜓</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Igarashi Kazuyoshi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>雷格西</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BEASTARS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Legoshi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>奥托·苏文</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Otto Suwen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>利欧</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rio</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>重本浩司</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shigemoto Kōji</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>常盘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>去参加联谊，却发现完全没有女生在场</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tokiwa</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>堀江一真</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>黑田崇矢</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>武内骏辅</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>岩中睦树</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>户谷菊之介</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>平川大辅</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>深町寿成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小林亲弘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小山力也</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -8797,10 +9129,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I768"/>
+  <dimension ref="A1:I799"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A739" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C764" sqref="C764"/>
+    <sheetView tabSelected="1" topLeftCell="A776" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E793" sqref="E793"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -25110,11 +25442,631 @@
       <c r="D768" s="1" t="s">
         <v>2457</v>
       </c>
-      <c r="F768" s="5">
+      <c r="F768" s="1">
         <v>2013</v>
       </c>
-      <c r="G768" s="5">
+      <c r="G768" s="1">
         <v>1</v>
+      </c>
+    </row>
+    <row r="769" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A769" s="1" t="s">
+        <v>2480</v>
+      </c>
+      <c r="B769" s="1" t="s">
+        <v>2374</v>
+      </c>
+      <c r="C769" s="1" t="s">
+        <v>1642</v>
+      </c>
+      <c r="D769" s="1" t="s">
+        <v>2481</v>
+      </c>
+      <c r="F769" s="1">
+        <v>2024</v>
+      </c>
+      <c r="G769" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="770" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A770" s="1" t="s">
+        <v>2482</v>
+      </c>
+      <c r="B770" s="1" t="s">
+        <v>2379</v>
+      </c>
+      <c r="C770" s="1" t="s">
+        <v>1959</v>
+      </c>
+      <c r="D770" s="1" t="s">
+        <v>2483</v>
+      </c>
+      <c r="F770" s="1">
+        <v>2024</v>
+      </c>
+      <c r="G770" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="771" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A771" s="1" t="s">
+        <v>2484</v>
+      </c>
+      <c r="B771" s="1" t="s">
+        <v>2382</v>
+      </c>
+      <c r="C771" s="1" t="s">
+        <v>2554</v>
+      </c>
+      <c r="D771" s="1" t="s">
+        <v>2485</v>
+      </c>
+      <c r="F771" s="1">
+        <v>2008</v>
+      </c>
+      <c r="G771" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="772" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A772" s="1" t="s">
+        <v>2486</v>
+      </c>
+      <c r="B772" s="1" t="s">
+        <v>2487</v>
+      </c>
+      <c r="C772" s="1" t="s">
+        <v>1960</v>
+      </c>
+      <c r="D772" s="1" t="s">
+        <v>2488</v>
+      </c>
+      <c r="F772" s="1">
+        <v>2023</v>
+      </c>
+      <c r="G772" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="773" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A773" s="1" t="s">
+        <v>2489</v>
+      </c>
+      <c r="B773" s="1" t="s">
+        <v>2490</v>
+      </c>
+      <c r="C773" s="1" t="s">
+        <v>1716</v>
+      </c>
+      <c r="D773" s="1" t="s">
+        <v>2491</v>
+      </c>
+      <c r="F773" s="1">
+        <v>2006</v>
+      </c>
+      <c r="G773" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="774" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A774" s="1" t="s">
+        <v>2492</v>
+      </c>
+      <c r="B774" s="1" t="s">
+        <v>2468</v>
+      </c>
+      <c r="C774" s="1" t="s">
+        <v>1626</v>
+      </c>
+      <c r="D774" s="1" t="s">
+        <v>2493</v>
+      </c>
+      <c r="F774" s="1">
+        <v>1989</v>
+      </c>
+      <c r="G774" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="775" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A775" s="1" t="s">
+        <v>2494</v>
+      </c>
+      <c r="B775" s="1" t="s">
+        <v>2495</v>
+      </c>
+      <c r="C775" s="1" t="s">
+        <v>2555</v>
+      </c>
+      <c r="D775" s="1" t="s">
+        <v>2496</v>
+      </c>
+      <c r="F775" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G775" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="776" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A776" s="1" t="s">
+        <v>2497</v>
+      </c>
+      <c r="B776" s="1" t="s">
+        <v>2498</v>
+      </c>
+      <c r="C776" s="1" t="s">
+        <v>2556</v>
+      </c>
+      <c r="D776" s="1" t="s">
+        <v>2499</v>
+      </c>
+      <c r="F776" s="1">
+        <v>2024</v>
+      </c>
+      <c r="G776" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="777" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A777" s="1" t="s">
+        <v>2500</v>
+      </c>
+      <c r="B777" s="1" t="s">
+        <v>2434</v>
+      </c>
+      <c r="C777" s="1" t="s">
+        <v>2557</v>
+      </c>
+      <c r="D777" s="1" t="s">
+        <v>2501</v>
+      </c>
+      <c r="F777" s="1">
+        <v>2024</v>
+      </c>
+      <c r="G777" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="778" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A778" s="1" t="s">
+        <v>2502</v>
+      </c>
+      <c r="B778" s="1" t="s">
+        <v>2443</v>
+      </c>
+      <c r="C778" s="1" t="s">
+        <v>1582</v>
+      </c>
+      <c r="D778" s="1" t="s">
+        <v>2503</v>
+      </c>
+      <c r="F778" s="1">
+        <v>2024</v>
+      </c>
+      <c r="G778" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="779" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A779" s="1" t="s">
+        <v>2504</v>
+      </c>
+      <c r="B779" s="1" t="s">
+        <v>2379</v>
+      </c>
+      <c r="C779" s="1" t="s">
+        <v>1616</v>
+      </c>
+      <c r="D779" s="1" t="s">
+        <v>2505</v>
+      </c>
+      <c r="F779" s="1">
+        <v>2024</v>
+      </c>
+      <c r="G779" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="780" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A780" s="1" t="s">
+        <v>2506</v>
+      </c>
+      <c r="B780" s="1" t="s">
+        <v>2406</v>
+      </c>
+      <c r="C780" s="1" t="s">
+        <v>1950</v>
+      </c>
+      <c r="D780" s="1" t="s">
+        <v>2507</v>
+      </c>
+      <c r="F780" s="1">
+        <v>2024</v>
+      </c>
+      <c r="G780" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="781" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A781" s="1" t="s">
+        <v>2508</v>
+      </c>
+      <c r="B781" s="1" t="s">
+        <v>2396</v>
+      </c>
+      <c r="C781" s="1" t="s">
+        <v>1620</v>
+      </c>
+      <c r="D781" s="1" t="s">
+        <v>2509</v>
+      </c>
+      <c r="F781" s="1">
+        <v>2024</v>
+      </c>
+      <c r="G781" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="782" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A782" s="1" t="s">
+        <v>2510</v>
+      </c>
+      <c r="B782" s="1" t="s">
+        <v>2386</v>
+      </c>
+      <c r="C782" s="1" t="s">
+        <v>1961</v>
+      </c>
+      <c r="D782" s="1" t="s">
+        <v>2511</v>
+      </c>
+      <c r="F782" s="1">
+        <v>2024</v>
+      </c>
+      <c r="G782" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="783" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A783" s="1" t="s">
+        <v>2512</v>
+      </c>
+      <c r="B783" s="1" t="s">
+        <v>2434</v>
+      </c>
+      <c r="C783" s="1" t="s">
+        <v>1616</v>
+      </c>
+      <c r="D783" s="1" t="s">
+        <v>2513</v>
+      </c>
+      <c r="F783" s="1">
+        <v>2024</v>
+      </c>
+      <c r="G783" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="784" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A784" s="1" t="s">
+        <v>2514</v>
+      </c>
+      <c r="B784" s="1" t="s">
+        <v>2515</v>
+      </c>
+      <c r="C784" s="1" t="s">
+        <v>2303</v>
+      </c>
+      <c r="D784" s="1" t="s">
+        <v>2516</v>
+      </c>
+      <c r="F784" s="1">
+        <v>2024</v>
+      </c>
+      <c r="G784" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="785" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A785" s="1" t="s">
+        <v>2517</v>
+      </c>
+      <c r="B785" s="1" t="s">
+        <v>2422</v>
+      </c>
+      <c r="C785" s="1" t="s">
+        <v>2558</v>
+      </c>
+      <c r="D785" s="1" t="s">
+        <v>2518</v>
+      </c>
+      <c r="F785" s="1">
+        <v>2024</v>
+      </c>
+      <c r="G785" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="786" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A786" s="1" t="s">
+        <v>2519</v>
+      </c>
+      <c r="B786" s="1" t="s">
+        <v>2393</v>
+      </c>
+      <c r="C786" s="1" t="s">
+        <v>2303</v>
+      </c>
+      <c r="D786" s="1" t="s">
+        <v>2520</v>
+      </c>
+      <c r="F786" s="1">
+        <v>2024</v>
+      </c>
+      <c r="G786" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="787" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A787" s="1" t="s">
+        <v>2521</v>
+      </c>
+      <c r="B787" s="1" t="s">
+        <v>2522</v>
+      </c>
+      <c r="C787" s="1" t="s">
+        <v>1705</v>
+      </c>
+      <c r="D787" s="1" t="s">
+        <v>2523</v>
+      </c>
+      <c r="F787" s="1">
+        <v>2024</v>
+      </c>
+      <c r="G787" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="788" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A788" s="1" t="s">
+        <v>2524</v>
+      </c>
+      <c r="B788" s="1" t="s">
+        <v>2414</v>
+      </c>
+      <c r="C788" s="1" t="s">
+        <v>2559</v>
+      </c>
+      <c r="D788" s="1" t="s">
+        <v>2525</v>
+      </c>
+      <c r="F788" s="1">
+        <v>2024</v>
+      </c>
+      <c r="G788" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="789" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A789" s="1" t="s">
+        <v>2526</v>
+      </c>
+      <c r="B789" s="1" t="s">
+        <v>2428</v>
+      </c>
+      <c r="C789" s="1" t="s">
+        <v>2560</v>
+      </c>
+      <c r="D789" s="1" t="s">
+        <v>2527</v>
+      </c>
+      <c r="F789" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G789" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="790" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A790" s="1" t="s">
+        <v>2528</v>
+      </c>
+      <c r="B790" s="1" t="s">
+        <v>2529</v>
+      </c>
+      <c r="C790" s="1" t="s">
+        <v>2312</v>
+      </c>
+      <c r="D790" s="1" t="s">
+        <v>2530</v>
+      </c>
+      <c r="F790" s="1">
+        <v>2024</v>
+      </c>
+      <c r="G790" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="791" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A791" s="1" t="s">
+        <v>2531</v>
+      </c>
+      <c r="B791" s="1" t="s">
+        <v>2437</v>
+      </c>
+      <c r="C791" s="1" t="s">
+        <v>1716</v>
+      </c>
+      <c r="D791" s="1" t="s">
+        <v>2532</v>
+      </c>
+      <c r="F791" s="1">
+        <v>2024</v>
+      </c>
+      <c r="G791" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="792" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A792" s="1" t="s">
+        <v>2533</v>
+      </c>
+      <c r="B792" s="1" t="s">
+        <v>2534</v>
+      </c>
+      <c r="C792" s="1" t="s">
+        <v>2303</v>
+      </c>
+      <c r="D792" s="1" t="s">
+        <v>2535</v>
+      </c>
+      <c r="F792" s="1">
+        <v>2024</v>
+      </c>
+      <c r="G792" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="793" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A793" s="1" t="s">
+        <v>2536</v>
+      </c>
+      <c r="B793" s="1" t="s">
+        <v>2537</v>
+      </c>
+      <c r="C793" s="1" t="s">
+        <v>1721</v>
+      </c>
+      <c r="D793" s="1" t="s">
+        <v>2538</v>
+      </c>
+      <c r="F793" s="1">
+        <v>2023</v>
+      </c>
+      <c r="G793" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="794" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A794" s="1" t="s">
+        <v>2539</v>
+      </c>
+      <c r="B794" s="1" t="s">
+        <v>2540</v>
+      </c>
+      <c r="C794" s="1" t="s">
+        <v>1652</v>
+      </c>
+      <c r="D794" s="1" t="s">
+        <v>2541</v>
+      </c>
+      <c r="F794" s="1">
+        <v>2024</v>
+      </c>
+      <c r="G794" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="795" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A795" s="1" t="s">
+        <v>2542</v>
+      </c>
+      <c r="B795" s="1" t="s">
+        <v>2543</v>
+      </c>
+      <c r="C795" s="1" t="s">
+        <v>2561</v>
+      </c>
+      <c r="D795" s="1" t="s">
+        <v>2544</v>
+      </c>
+      <c r="F795" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G795" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="796" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A796" s="1" t="s">
+        <v>2545</v>
+      </c>
+      <c r="B796" s="1" t="s">
+        <v>2431</v>
+      </c>
+      <c r="C796" s="1" t="s">
+        <v>2302</v>
+      </c>
+      <c r="D796" s="1" t="s">
+        <v>2546</v>
+      </c>
+      <c r="F796" s="1">
+        <v>2016</v>
+      </c>
+      <c r="G796" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="797" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A797" s="1" t="s">
+        <v>2547</v>
+      </c>
+      <c r="B797" s="1" t="s">
+        <v>2446</v>
+      </c>
+      <c r="C797" s="1" t="s">
+        <v>1650</v>
+      </c>
+      <c r="D797" s="1" t="s">
+        <v>2548</v>
+      </c>
+      <c r="F797" s="1">
+        <v>2021</v>
+      </c>
+      <c r="G797" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="798" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A798" s="1" t="s">
+        <v>2549</v>
+      </c>
+      <c r="B798" s="1" t="s">
+        <v>2440</v>
+      </c>
+      <c r="C798" s="1" t="s">
+        <v>2562</v>
+      </c>
+      <c r="D798" s="1" t="s">
+        <v>2550</v>
+      </c>
+      <c r="F798" s="1">
+        <v>2024</v>
+      </c>
+      <c r="G798" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="799" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A799" s="1" t="s">
+        <v>2551</v>
+      </c>
+      <c r="B799" s="1" t="s">
+        <v>2552</v>
+      </c>
+      <c r="C799" s="1" t="s">
+        <v>2556</v>
+      </c>
+      <c r="D799" s="1" t="s">
+        <v>2553</v>
+      </c>
+      <c r="F799" s="1">
+        <v>2024</v>
+      </c>
+      <c r="G799" s="1">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>